<commit_message>
updated Bulk CI and plaza features and steps
</commit_message>
<xml_diff>
--- a/src/test/resources/Test Attachments/5DuplicateCIs/5CIsXLSX.xlsx
+++ b/src/test/resources/Test Attachments/5DuplicateCIs/5CIsXLSX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahesh vaddegani\Downloads\Test Case Attachments 2\TemplatesForBulkCITests\5 CIs - Duplicated CI's\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\oneworkflow.automation\src\test\resources\Test Attachments\5DuplicateCIs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA06BF0-1DD0-409B-8B3E-E2667E382695}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25712EA1-607A-4B24-9955-4E1A162B7128}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>CI Name</t>
   </si>
@@ -392,61 +392,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>